<commit_message>
add: documentacion del requerimiento 8
</commit_message>
<xml_diff>
--- a/Docs/graficas.xlsx
+++ b/Docs/graficas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikteh\Desktop\U. DE VERDAD\Segundo Semestre\LABSEDA\Reto1-G01\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBC0D9A-2ECD-4E5E-8E01-04AA7DFE91E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9243B2C7-3249-4FE1-B21E-1AF4D31D703E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18D8D079-6A18-4ABB-8F7F-373E1F538B09}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
   <si>
     <t>Tiempo (ms)</t>
   </si>
@@ -1516,6 +1516,343 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t>Requerimiento 8</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$38:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>893817</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1843170</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2699180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3639811</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4628467</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$C$38:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FEC3-4861-B3ED-74FFBF46B012}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="235388912"/>
+        <c:axId val="235398064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="235388912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="235398064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="235398064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="235388912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1676,6 +2013,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3225,6 +3602,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3881,6 +4774,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9259C492-0874-485F-A343-B69DE54BAE14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4186,10 +5115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9439473F-057B-40D0-87E5-EC14A57AF5E5}">
-  <dimension ref="B2:O26"/>
+  <dimension ref="B2:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4369,6 +5298,54 @@
         <v>500000</v>
       </c>
     </row>
+    <row r="37" spans="2:3">
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="2">
+        <v>893817</v>
+      </c>
+      <c r="C38">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" s="2">
+        <v>1843170</v>
+      </c>
+      <c r="C39">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="1">
+        <v>2699180</v>
+      </c>
+      <c r="C40">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" s="2">
+        <v>3639811</v>
+      </c>
+      <c r="C41">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" s="2">
+        <v>4628467</v>
+      </c>
+      <c r="C42">
+        <v>500000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update: ajustes de algunos requerimientos y documentación
</commit_message>
<xml_diff>
--- a/Docs/graficas.xlsx
+++ b/Docs/graficas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f6ea73de10acc2f/Desktop/EDA/Reto_1/Reto1-G01/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikteh\Desktop\U. DE VERDAD\Segundo Semestre\LABSEDA\Reto1-G01\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{9243B2C7-3249-4FE1-B21E-1AF4D31D703E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2C08A1B-9F9B-4751-9268-F933B1372682}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB8484B-A574-4281-B507-8FF013C1F237}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{18D8D079-6A18-4ABB-8F7F-373E1F538B09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18D8D079-6A18-4ABB-8F7F-373E1F538B09}"/>
   </bookViews>
   <sheets>
     <sheet name="PRUEBAS AMD RYZEN 7 22 RAM" sheetId="1" r:id="rId1"/>
@@ -1975,6 +1975,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'PRUEBAS AMD RYZEN 7 22 RAM'!$B$38:$B$42</c:f>
@@ -1982,19 +1996,19 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>893817</c:v>
+                  <c:v>1150047</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1843170</c:v>
+                  <c:v>2524231</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2699180</c:v>
+                  <c:v>3260040</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3639811</c:v>
+                  <c:v>4533304</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4628467</c:v>
+                  <c:v>5719113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9334,9 +9348,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:colOff>600076</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9550,9 +9564,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -9590,7 +9604,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -9696,7 +9710,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -9838,7 +9852,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9848,15 +9862,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9439473F-057B-40D0-87E5-EC14A57AF5E5}">
   <dimension ref="B2:O42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="14" max="14" width="21.6640625" customWidth="1"/>
-    <col min="15" max="15" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15">
@@ -10039,7 +10053,7 @@
     </row>
     <row r="38" spans="2:3">
       <c r="B38" s="2">
-        <v>893817</v>
+        <v>1150047</v>
       </c>
       <c r="C38">
         <v>100000</v>
@@ -10047,7 +10061,7 @@
     </row>
     <row r="39" spans="2:3">
       <c r="B39" s="2">
-        <v>1843170</v>
+        <v>2524231</v>
       </c>
       <c r="C39">
         <v>200000</v>
@@ -10055,7 +10069,7 @@
     </row>
     <row r="40" spans="2:3">
       <c r="B40" s="1">
-        <v>2699180</v>
+        <v>3260040</v>
       </c>
       <c r="C40">
         <v>300000</v>
@@ -10063,7 +10077,7 @@
     </row>
     <row r="41" spans="2:3">
       <c r="B41" s="2">
-        <v>3639811</v>
+        <v>4533304</v>
       </c>
       <c r="C41">
         <v>400000</v>
@@ -10071,7 +10085,7 @@
     </row>
     <row r="42" spans="2:3">
       <c r="B42" s="2">
-        <v>4628467</v>
+        <v>5719113</v>
       </c>
       <c r="C42">
         <v>500000</v>
@@ -10088,17 +10102,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB5058C-02D9-46A9-9FFC-C4328BBC9163}">
   <dimension ref="B4:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R3" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView topLeftCell="J3" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.21875" customWidth="1"/>
-    <col min="21" max="21" width="16.5546875" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="21" max="21" width="16.5703125" customWidth="1"/>
     <col min="22" max="22" width="14" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>